<commit_message>
added pics, added new manual
</commit_message>
<xml_diff>
--- a/Manuals-Labels-BOM-REV-10/BOMs/REV-10-BOM.xlsx
+++ b/Manuals-Labels-BOM-REV-10/BOMs/REV-10-BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="404">
   <si>
     <t>QTY</t>
   </si>
@@ -718,10 +718,25 @@
     <t>https://www.digikey.com/en/products/detail/molex/0197084013/3183362</t>
   </si>
   <si>
-    <t>SCREW</t>
-  </si>
-  <si>
-    <t>#4-40x3/16” pan head thread-cutting screw</t>
+    <t>SCREW 1</t>
+  </si>
+  <si>
+    <t>Screws included with and for the Serpac Case</t>
+  </si>
+  <si>
+    <t>SR6005-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#4 x 3/8" </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/serpac/6005/307599</t>
+  </si>
+  <si>
+    <t>SCREW 2</t>
+  </si>
+  <si>
+    <t>#4-40x3/16” pan head thread-cutting screw (for mounting board)</t>
   </si>
   <si>
     <t>90087A105</t>
@@ -1256,11 +1271,11 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -1454,17 +1469,17 @@
     <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="12" fontId="5" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="12" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2764,7 +2779,7 @@
         <v>13.0</v>
       </c>
       <c r="H35" s="7">
-        <f t="shared" ref="H35:H46" si="5">G35*A35</f>
+        <f t="shared" ref="H35:H43" si="5">G35*A35</f>
         <v>13</v>
       </c>
       <c r="I35" s="4" t="s">
@@ -3032,46 +3047,38 @@
       <c r="K43" s="4"/>
     </row>
     <row r="44">
-      <c r="A44" s="7">
+      <c r="A44" s="15">
         <v>4.0</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="15" t="s">
         <v>235</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4" t="s">
+      <c r="D44" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="E44" s="15">
+        <v>6005.0</v>
+      </c>
+      <c r="F44" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="G44" s="7">
-        <v>0.1018</v>
-      </c>
-      <c r="H44" s="7">
-        <f t="shared" si="5"/>
-        <v>0.4072</v>
-      </c>
-      <c r="I44" s="4" t="s">
+      <c r="I44" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="J44" s="9" t="s">
+      <c r="J44" s="23" t="s">
         <v>239</v>
       </c>
       <c r="K44" s="4"/>
     </row>
     <row r="45">
       <c r="A45" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="B45" s="4" t="s">
+        <v>4.0</v>
+      </c>
+      <c r="B45" s="8" t="s">
         <v>240</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="8" t="s">
         <v>241</v>
       </c>
       <c r="E45" s="4" t="s">
@@ -3081,11 +3088,11 @@
         <v>242</v>
       </c>
       <c r="G45" s="7">
-        <v>0.467</v>
+        <v>0.1018</v>
       </c>
       <c r="H45" s="7">
-        <f t="shared" si="5"/>
-        <v>0.934</v>
+        <f t="shared" ref="H45:H47" si="6">G45*A45</f>
+        <v>0.4072</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>243</v>
@@ -3097,93 +3104,95 @@
     </row>
     <row r="46">
       <c r="A46" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="F46" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G46" s="7">
+        <v>0.467</v>
+      </c>
+      <c r="H46" s="7">
+        <f t="shared" si="6"/>
+        <v>0.934</v>
+      </c>
+      <c r="I46" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="J46" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="G46" s="7">
+      <c r="K46" s="4"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="G47" s="7">
         <v>0.8888</v>
       </c>
-      <c r="H46" s="7">
-        <f t="shared" si="5"/>
+      <c r="H47" s="7">
+        <f t="shared" si="6"/>
         <v>0.8888</v>
       </c>
-      <c r="I46" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="J46" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="K46" s="4"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="23"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23" t="s">
-        <v>252</v>
-      </c>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
+      <c r="I47" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="J47" s="9" t="s">
+        <v>256</v>
+      </c>
       <c r="K47" s="4"/>
     </row>
     <row r="48">
-      <c r="A48" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="G48" s="7">
-        <v>8.0</v>
-      </c>
-      <c r="H48" s="7">
-        <f t="shared" ref="H48:H50" si="6">G48*A48</f>
-        <v>8</v>
-      </c>
-      <c r="I48" s="4"/>
-      <c r="J48" s="9" t="s">
-        <v>256</v>
-      </c>
+      <c r="A48" s="24"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24"/>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24"/>
       <c r="K48" s="4"/>
     </row>
     <row r="49">
       <c r="A49" s="7">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>259</v>
@@ -3192,258 +3201,263 @@
         <v>260</v>
       </c>
       <c r="G49" s="7">
-        <v>0.75075</v>
+        <v>8.0</v>
       </c>
       <c r="H49" s="7">
-        <f t="shared" si="6"/>
-        <v>1.5015</v>
-      </c>
-      <c r="I49" s="4" t="s">
+        <f t="shared" ref="H49:H51" si="7">G49*A49</f>
+        <v>8</v>
+      </c>
+      <c r="I49" s="4"/>
+      <c r="J49" s="9" t="s">
         <v>261</v>
-      </c>
-      <c r="J49" s="9" t="s">
-        <v>262</v>
       </c>
       <c r="K49" s="4"/>
     </row>
     <row r="50">
       <c r="A50" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="E50" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="G50" s="7">
+        <v>0.75075</v>
+      </c>
+      <c r="H50" s="7">
+        <f t="shared" si="7"/>
+        <v>1.5015</v>
+      </c>
+      <c r="I50" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="F50" s="4" t="s">
+      <c r="J50" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="G50" s="7">
+      <c r="K50" s="4"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="G51" s="7">
         <v>1.0443</v>
       </c>
-      <c r="H50" s="7">
-        <f t="shared" si="6"/>
+      <c r="H51" s="7">
+        <f t="shared" si="7"/>
         <v>1.0443</v>
       </c>
-      <c r="I50" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="J50" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="K50" s="4"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>271</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="G51" s="15" t="s">
+      <c r="I51" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="I51" s="15" t="s">
+      <c r="J51" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="J51" s="15" t="s">
+      <c r="K51" s="4"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="B52" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="K51" s="4"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="24"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24" t="s">
+      <c r="D52" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
+      <c r="E52" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="G52" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="I52" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="J52" s="15" t="s">
+        <v>280</v>
+      </c>
       <c r="K52" s="4"/>
     </row>
     <row r="53">
-      <c r="A53" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="7">
-        <v>0.8014</v>
-      </c>
-      <c r="H53" s="7">
-        <f t="shared" ref="H53:H62" si="7">G53*A53</f>
-        <v>0.8014</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="J53" s="9" t="s">
-        <v>280</v>
-      </c>
+      <c r="A53" s="25"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
       <c r="K53" s="4"/>
     </row>
     <row r="54">
       <c r="A54" s="7">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="7">
-        <v>0.083</v>
+        <v>0.8014</v>
       </c>
       <c r="H54" s="7">
-        <f t="shared" si="7"/>
-        <v>0.581</v>
+        <f t="shared" ref="H54:H63" si="8">G54*A54</f>
+        <v>0.8014</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="K54" s="4"/>
     </row>
     <row r="55">
       <c r="A55" s="7">
-        <v>27.0</v>
+        <v>7.0</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="7">
-        <v>0.01299</v>
+        <v>0.083</v>
       </c>
       <c r="H55" s="7">
-        <f t="shared" si="7"/>
-        <v>0.35073</v>
+        <f t="shared" si="8"/>
+        <v>0.581</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="K55" s="4"/>
     </row>
     <row r="56">
       <c r="A56" s="7">
-        <v>1.0</v>
+        <v>27.0</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="7">
-        <v>0.17</v>
+        <v>0.01299</v>
       </c>
       <c r="H56" s="7">
-        <f t="shared" si="7"/>
-        <v>0.17</v>
+        <f t="shared" si="8"/>
+        <v>0.35073</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="K56" s="4"/>
     </row>
     <row r="57">
-      <c r="A57" s="10">
-        <v>26.0</v>
+      <c r="A57" s="7">
+        <v>1.0</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C57" s="4"/>
-      <c r="D57" s="8" t="s">
-        <v>294</v>
+      <c r="D57" s="4" t="s">
+        <v>295</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="8">
+      <c r="G57" s="7">
+        <v>0.17</v>
+      </c>
+      <c r="H57" s="7">
+        <f t="shared" si="8"/>
+        <v>0.17</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="J57" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="K57" s="4"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="10">
+        <v>26.0</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="8">
         <v>0.02</v>
       </c>
-      <c r="H57" s="7">
-        <f t="shared" si="7"/>
+      <c r="H58" s="7">
+        <f t="shared" si="8"/>
         <v>0.52</v>
       </c>
-      <c r="I57" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="J57" s="25" t="s">
-        <v>296</v>
-      </c>
-      <c r="K57" s="4"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>297</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="G58" s="15">
-        <v>0.13</v>
-      </c>
-      <c r="H58" s="7">
-        <f t="shared" si="7"/>
-        <v>0.13</v>
-      </c>
-      <c r="I58" s="15" t="s">
-        <v>299</v>
+      <c r="I58" s="8" t="s">
+        <v>300</v>
       </c>
       <c r="J58" s="26" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="59">
@@ -3451,160 +3465,155 @@
         <v>1.0</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G59" s="15">
-        <v>0.17</v>
+        <v>0.13</v>
       </c>
       <c r="H59" s="7">
-        <f t="shared" si="7"/>
-        <v>0.17</v>
+        <f t="shared" si="8"/>
+        <v>0.13</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="J59" s="26" t="s">
         <v>304</v>
+      </c>
+      <c r="J59" s="23" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="15">
-        <v>14.0</v>
+        <v>1.0</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G60" s="15">
-        <v>0.15</v>
+        <v>0.17</v>
       </c>
       <c r="H60" s="7">
-        <f t="shared" si="7"/>
-        <v>2.1</v>
+        <f t="shared" si="8"/>
+        <v>0.17</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>303</v>
+        <v>308</v>
+      </c>
+      <c r="J60" s="23" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="15">
-        <v>2.0</v>
+        <v>14.0</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D61" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="G61" s="15">
+        <v>0.15</v>
+      </c>
+      <c r="H61" s="7">
+        <f t="shared" si="8"/>
+        <v>2.1</v>
+      </c>
+      <c r="I61" s="15" t="s">
         <v>308</v>
-      </c>
-      <c r="G61" s="15">
-        <v>0.02</v>
-      </c>
-      <c r="H61" s="7">
-        <f t="shared" si="7"/>
-        <v>0.04</v>
-      </c>
-      <c r="I61" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="J61" s="26" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="15">
+        <v>2.0</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="G62" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="H62" s="7">
+        <f t="shared" si="8"/>
+        <v>0.04</v>
+      </c>
+      <c r="I62" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="J62" s="23" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="15">
         <v>7.0</v>
       </c>
-      <c r="B62" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="G62" s="15">
+      <c r="B63" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="G63" s="15">
         <v>0.03</v>
       </c>
-      <c r="H62" s="7">
-        <f t="shared" si="7"/>
+      <c r="H63" s="7">
+        <f t="shared" si="8"/>
         <v>0.21</v>
       </c>
-      <c r="I62" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="J62" s="26" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="27"/>
-      <c r="B64" s="27"/>
-      <c r="C64" s="27"/>
-      <c r="D64" s="28" t="s">
-        <v>315</v>
-      </c>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="27"/>
-      <c r="I64" s="27"/>
-      <c r="J64" s="27"/>
+      <c r="I63" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="J63" s="23" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
+      <c r="A65" s="27"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="28" t="s">
+        <v>320</v>
+      </c>
+      <c r="E65" s="27"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="27"/>
+      <c r="I65" s="27"/>
+      <c r="J65" s="27"/>
     </row>
     <row r="66">
-      <c r="A66" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B66" s="8" t="s">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B67" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C67" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="G66" s="7">
-        <v>0.0316</v>
-      </c>
-      <c r="I66" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="J66" s="9" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>19</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>322</v>
@@ -3616,82 +3625,82 @@
         <v>324</v>
       </c>
       <c r="G67" s="7">
-        <v>0.013</v>
+        <v>0.0316</v>
       </c>
       <c r="I67" s="15" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="7">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G68" s="7">
-        <v>0.01</v>
-      </c>
-      <c r="I68" s="29" t="s">
-        <v>320</v>
+        <v>0.013</v>
+      </c>
+      <c r="I68" s="15" t="s">
+        <v>325</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="7">
         <v>1.0</v>
       </c>
-      <c r="B69" s="29" t="s">
-        <v>30</v>
+      <c r="B69" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="G69" s="7">
         <v>0.01</v>
       </c>
       <c r="I69" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="7">
         <v>1.0</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>334</v>
+      <c r="B70" s="29" t="s">
+        <v>30</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>335</v>
@@ -3703,10 +3712,10 @@
         <v>337</v>
       </c>
       <c r="G70" s="7">
-        <v>0.013</v>
+        <v>0.01</v>
       </c>
       <c r="I70" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J70" s="9" t="s">
         <v>338</v>
@@ -3720,7 +3729,7 @@
         <v>339</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>340</v>
@@ -3732,10 +3741,10 @@
         <v>342</v>
       </c>
       <c r="G71" s="7">
-        <v>0.017</v>
+        <v>0.013</v>
       </c>
       <c r="I71" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J71" s="9" t="s">
         <v>343</v>
@@ -3749,7 +3758,7 @@
         <v>344</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>345</v>
@@ -3764,21 +3773,21 @@
         <v>0.017</v>
       </c>
       <c r="I72" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J72" s="9" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="10">
-        <v>2.0</v>
+      <c r="A73" s="7">
+        <v>1.0</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>349</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>350</v>
@@ -3790,24 +3799,24 @@
         <v>352</v>
       </c>
       <c r="G73" s="7">
-        <v>0.01</v>
+        <v>0.017</v>
       </c>
       <c r="I73" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J73" s="9" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="7">
-        <v>1.0</v>
+      <c r="A74" s="10">
+        <v>2.0</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>354</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>355</v>
@@ -3819,11 +3828,10 @@
         <v>357</v>
       </c>
       <c r="G74" s="7">
-        <v>0.011</v>
-      </c>
-      <c r="H74" s="4"/>
+        <v>0.01</v>
+      </c>
       <c r="I74" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J74" s="9" t="s">
         <v>358</v>
@@ -3837,7 +3845,7 @@
         <v>359</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>360</v>
@@ -3851,8 +3859,9 @@
       <c r="G75" s="7">
         <v>0.011</v>
       </c>
+      <c r="H75" s="4"/>
       <c r="I75" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J75" s="9" t="s">
         <v>363</v>
@@ -3866,7 +3875,7 @@
         <v>364</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>365</v>
@@ -3878,10 +3887,10 @@
         <v>367</v>
       </c>
       <c r="G76" s="7">
-        <v>0.0104</v>
+        <v>0.011</v>
       </c>
       <c r="I76" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J76" s="9" t="s">
         <v>368</v>
@@ -3894,99 +3903,99 @@
       <c r="B77" s="4" t="s">
         <v>369</v>
       </c>
-      <c r="C77" s="29" t="s">
-        <v>76</v>
+      <c r="C77" s="8" t="s">
+        <v>71</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>370</v>
       </c>
       <c r="E77" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="G77" s="7">
+        <v>0.0104</v>
+      </c>
+      <c r="I77" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="J77" s="9" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="C78" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="E78" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F77" s="4" t="s">
+      <c r="F78" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G77" s="7">
+      <c r="G78" s="7">
         <v>0.7575</v>
       </c>
-      <c r="I77" s="29" t="s">
+      <c r="I78" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="J77" s="9" t="s">
+      <c r="J78" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="12"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="12"/>
-    </row>
     <row r="79">
-      <c r="A79" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="B79" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D79" s="30" t="s">
-        <v>372</v>
-      </c>
-      <c r="E79" s="30" t="s">
-        <v>373</v>
-      </c>
-      <c r="F79" s="30" t="s">
-        <v>374</v>
-      </c>
-      <c r="G79" s="30">
-        <v>0.059</v>
-      </c>
-      <c r="I79" s="29" t="s">
-        <v>320</v>
-      </c>
-      <c r="J79" s="31" t="s">
-        <v>375</v>
-      </c>
+      <c r="A79" s="12"/>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
       <c r="K79" s="4"/>
     </row>
     <row r="80">
       <c r="A80" s="30">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B80" s="30" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D80" s="30" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F80" s="30" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G80" s="30">
-        <v>0.119</v>
+        <v>0.059</v>
       </c>
       <c r="I80" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J80" s="31" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="K80" s="4"/>
     </row>
@@ -3994,29 +4003,29 @@
       <c r="A81" s="30">
         <v>1.0</v>
       </c>
-      <c r="B81" s="15" t="s">
-        <v>96</v>
+      <c r="B81" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D81" s="30" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F81" s="30" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G81" s="30">
         <v>0.119</v>
       </c>
       <c r="I81" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J81" s="31" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K81" s="4"/>
     </row>
@@ -4025,57 +4034,57 @@
         <v>1.0</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D82" s="30" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="F82" s="30" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G82" s="30">
-        <v>0.138</v>
+        <v>0.119</v>
       </c>
       <c r="I82" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J82" s="31" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="30">
         <v>1.0</v>
       </c>
-      <c r="B83" s="30" t="s">
-        <v>110</v>
+      <c r="B83" s="15" t="s">
+        <v>103</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D83" s="30" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="F83" s="30" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="G83" s="30">
-        <v>0.086</v>
+        <v>0.138</v>
       </c>
       <c r="I83" s="29" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="J83" s="31" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="84">
@@ -4083,57 +4092,86 @@
         <v>1.0</v>
       </c>
       <c r="B84" s="30" t="s">
-        <v>392</v>
-      </c>
-      <c r="C84" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D84" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="E84" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="F84" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="G84" s="30">
+        <v>0.086</v>
+      </c>
+      <c r="I84" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="J84" s="31" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="30">
+        <v>1.0</v>
+      </c>
+      <c r="B85" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="C85" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D84" s="30" t="s">
-        <v>380</v>
-      </c>
-      <c r="E84" s="30" t="s">
-        <v>381</v>
-      </c>
-      <c r="F84" s="30" t="s">
-        <v>382</v>
-      </c>
-      <c r="G84" s="30">
+      <c r="D85" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="E85" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="F85" s="30" t="s">
+        <v>387</v>
+      </c>
+      <c r="G85" s="30">
         <v>0.119</v>
       </c>
-      <c r="I84" s="29" t="s">
-        <v>320</v>
-      </c>
-      <c r="J84" s="31" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="B85" s="15" t="s">
-        <v>393</v>
-      </c>
-      <c r="C85" s="15" t="s">
+      <c r="I85" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="J85" s="31" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="15">
+        <v>1.0</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>398</v>
+      </c>
+      <c r="C86" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D85" s="15" t="s">
-        <v>394</v>
-      </c>
-      <c r="E85" s="15" t="s">
-        <v>395</v>
-      </c>
-      <c r="F85" s="15" t="s">
-        <v>396</v>
-      </c>
-      <c r="G85" s="15">
+      <c r="D86" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="E86" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="F86" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="G86" s="15">
         <v>0.2079</v>
       </c>
-      <c r="I85" s="15" t="s">
-        <v>397</v>
-      </c>
-      <c r="J85" s="16" t="s">
-        <v>398</v>
+      <c r="I86" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="J86" s="16" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="91">
@@ -4297,19 +4335,19 @@
     <hyperlink r:id="rId37" ref="J44"/>
     <hyperlink r:id="rId38" ref="J45"/>
     <hyperlink r:id="rId39" ref="J46"/>
-    <hyperlink r:id="rId40" ref="J48"/>
+    <hyperlink r:id="rId40" ref="J47"/>
     <hyperlink r:id="rId41" ref="J49"/>
     <hyperlink r:id="rId42" ref="J50"/>
-    <hyperlink r:id="rId43" ref="J53"/>
+    <hyperlink r:id="rId43" ref="J51"/>
     <hyperlink r:id="rId44" ref="J54"/>
     <hyperlink r:id="rId45" ref="J55"/>
     <hyperlink r:id="rId46" ref="J56"/>
     <hyperlink r:id="rId47" ref="J57"/>
     <hyperlink r:id="rId48" ref="J58"/>
     <hyperlink r:id="rId49" ref="J59"/>
-    <hyperlink r:id="rId50" ref="J61"/>
+    <hyperlink r:id="rId50" ref="J60"/>
     <hyperlink r:id="rId51" ref="J62"/>
-    <hyperlink r:id="rId52" ref="J66"/>
+    <hyperlink r:id="rId52" ref="J63"/>
     <hyperlink r:id="rId53" ref="J67"/>
     <hyperlink r:id="rId54" ref="J68"/>
     <hyperlink r:id="rId55" ref="J69"/>
@@ -4321,17 +4359,18 @@
     <hyperlink r:id="rId61" ref="J75"/>
     <hyperlink r:id="rId62" ref="J76"/>
     <hyperlink r:id="rId63" ref="J77"/>
-    <hyperlink r:id="rId64" ref="J79"/>
+    <hyperlink r:id="rId64" ref="J78"/>
     <hyperlink r:id="rId65" ref="J80"/>
     <hyperlink r:id="rId66" ref="J81"/>
     <hyperlink r:id="rId67" ref="J82"/>
     <hyperlink r:id="rId68" ref="J83"/>
     <hyperlink r:id="rId69" ref="J84"/>
     <hyperlink r:id="rId70" ref="J85"/>
+    <hyperlink r:id="rId71" ref="J86"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId71"/>
+  <drawing r:id="rId72"/>
 </worksheet>
 </file>
</xml_diff>